<commit_message>
agrego caso de prueba login ejemplo
</commit_message>
<xml_diff>
--- a/Matriz de trazabilidad.xlsx
+++ b/Matriz de trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kage Bushin No Jutsu\Desktop\QA-autom1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9172C0D6-6292-4B93-8E55-8535ECE4BAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9797DEA9-37F3-49F4-8886-4B95C9E1C110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D6194902-CC72-4C6D-8D7A-E5F84B4A5EE8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>ID REQUISITO</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Caso de prueba copia de seguridad quincenal</t>
+  </si>
+  <si>
+    <t>RQ004</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir upload de documentos</t>
+  </si>
+  <si>
+    <t>Caso de prueba upload recetas</t>
+  </si>
+  <si>
+    <t>Disenio del sistema de almacenamiento</t>
   </si>
 </sst>
 </file>
@@ -467,17 +479,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A901B045-C2FB-4B77-B5B6-044737CCE0A9}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="88.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -557,6 +569,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>